<commit_message>
fix error occured on empty row or cell skipped in xml
</commit_message>
<xml_diff>
--- a/examples/sample.xlsx
+++ b/examples/sample.xlsx
@@ -27,10 +27,26 @@
     <t>Itsuki1</t>
   </si>
   <si>
-    <t>itsuki2</t>
-  </si>
-  <si>
-    <t>itsuki3</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>hlink_inside</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>hlink_outside</t>
+    </r>
   </si>
   <si>
     <t>itsuki4+
@@ -83,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -96,6 +112,12 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -506,10 +528,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1647,6 +1669,10 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B6:B7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" location="'Sheet 2 - Custom grid lines'!R2C1" tooltip="" display="hlink_inside"/>
+    <hyperlink ref="B5" r:id="rId1" location="" tooltip="" display="hlink_outside"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>